<commit_message>
GitHub Action: commit results of ci-schema-convert workflow
</commit_message>
<xml_diff>
--- a/model_templates/ark.BDMFCSFileAnnotations.xlsx
+++ b/model_templates/ark.BDMFCSFileAnnotations.xlsx
@@ -52847,22 +52847,22 @@
       <formula>$R1 = "AMP RA/SLE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U1000">
+  <conditionalFormatting sqref="T1:T1000">
     <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>$F1 = "single specimen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T1:T1000">
+  <conditionalFormatting sqref="U1:U1000">
     <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>$F1 = "single specimen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q1000">
+  <conditionalFormatting sqref="P1:P1000">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>$F1 = "multispecimen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1000">
+  <conditionalFormatting sqref="Q1:Q1000">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>$F1 = "multispecimen"</formula>
     </cfRule>

</xml_diff>